<commit_message>
teste dans le main et modif dans pyromancien
</commit_message>
<xml_diff>
--- a/planning.xlsx
+++ b/planning.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:11_{7BFB9A4D-E791-4EFF-A64B-F3F6C4CEA54A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38563C21-A25F-4751-8E58-2C7568DB1A13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="48">
   <si>
     <t>Créez un planning de projet dans cette feuille de calcul.
 Entrez le titre de ce projet dans la cellule B1. 
@@ -219,6 +219,9 @@
   </si>
   <si>
     <t>Arthur</t>
+  </si>
+  <si>
+    <t>Baptiste+Théo</t>
   </si>
 </sst>
 </file>
@@ -1159,6 +1162,9 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="8">
       <alignment horizontal="right" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyProtection="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="168" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -1170,9 +1176,6 @@
     </xf>
     <xf numFmtId="166" fontId="7" fillId="0" borderId="3" xfId="9">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyProtection="1">
-      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="54">
@@ -1785,7 +1788,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
+      <selection pane="bottomLeft" activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1817,7 +1820,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="35"/>
-      <c r="H2" s="66"/>
+      <c r="H2" s="62"/>
     </row>
     <row r="3" spans="1:63" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="30" t="s">
@@ -1827,10 +1830,10 @@
       <c r="C3" s="61" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="65">
+      <c r="D3" s="66">
         <v>45763</v>
       </c>
-      <c r="E3" s="65"/>
+      <c r="E3" s="66"/>
     </row>
     <row r="4" spans="1:63" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="31" t="s">
@@ -1842,86 +1845,86 @@
       <c r="D4" s="7">
         <v>1</v>
       </c>
-      <c r="H4" s="62">
+      <c r="H4" s="63">
         <f>H5</f>
         <v>45761</v>
       </c>
-      <c r="I4" s="63"/>
-      <c r="J4" s="63"/>
-      <c r="K4" s="63"/>
-      <c r="L4" s="63"/>
-      <c r="M4" s="63"/>
-      <c r="N4" s="64"/>
-      <c r="O4" s="62">
+      <c r="I4" s="64"/>
+      <c r="J4" s="64"/>
+      <c r="K4" s="64"/>
+      <c r="L4" s="64"/>
+      <c r="M4" s="64"/>
+      <c r="N4" s="65"/>
+      <c r="O4" s="63">
         <f>O5</f>
         <v>45768</v>
       </c>
-      <c r="P4" s="63"/>
-      <c r="Q4" s="63"/>
-      <c r="R4" s="63"/>
-      <c r="S4" s="63"/>
-      <c r="T4" s="63"/>
-      <c r="U4" s="64"/>
-      <c r="V4" s="62">
+      <c r="P4" s="64"/>
+      <c r="Q4" s="64"/>
+      <c r="R4" s="64"/>
+      <c r="S4" s="64"/>
+      <c r="T4" s="64"/>
+      <c r="U4" s="65"/>
+      <c r="V4" s="63">
         <f>V5</f>
         <v>45775</v>
       </c>
-      <c r="W4" s="63"/>
-      <c r="X4" s="63"/>
-      <c r="Y4" s="63"/>
-      <c r="Z4" s="63"/>
-      <c r="AA4" s="63"/>
-      <c r="AB4" s="64"/>
-      <c r="AC4" s="62">
+      <c r="W4" s="64"/>
+      <c r="X4" s="64"/>
+      <c r="Y4" s="64"/>
+      <c r="Z4" s="64"/>
+      <c r="AA4" s="64"/>
+      <c r="AB4" s="65"/>
+      <c r="AC4" s="63">
         <f>AC5</f>
         <v>45782</v>
       </c>
-      <c r="AD4" s="63"/>
-      <c r="AE4" s="63"/>
-      <c r="AF4" s="63"/>
-      <c r="AG4" s="63"/>
-      <c r="AH4" s="63"/>
-      <c r="AI4" s="64"/>
-      <c r="AJ4" s="62">
+      <c r="AD4" s="64"/>
+      <c r="AE4" s="64"/>
+      <c r="AF4" s="64"/>
+      <c r="AG4" s="64"/>
+      <c r="AH4" s="64"/>
+      <c r="AI4" s="65"/>
+      <c r="AJ4" s="63">
         <f>AJ5</f>
         <v>45789</v>
       </c>
-      <c r="AK4" s="63"/>
-      <c r="AL4" s="63"/>
-      <c r="AM4" s="63"/>
-      <c r="AN4" s="63"/>
-      <c r="AO4" s="63"/>
-      <c r="AP4" s="64"/>
-      <c r="AQ4" s="62">
+      <c r="AK4" s="64"/>
+      <c r="AL4" s="64"/>
+      <c r="AM4" s="64"/>
+      <c r="AN4" s="64"/>
+      <c r="AO4" s="64"/>
+      <c r="AP4" s="65"/>
+      <c r="AQ4" s="63">
         <f>AQ5</f>
         <v>45796</v>
       </c>
-      <c r="AR4" s="63"/>
-      <c r="AS4" s="63"/>
-      <c r="AT4" s="63"/>
-      <c r="AU4" s="63"/>
-      <c r="AV4" s="63"/>
-      <c r="AW4" s="64"/>
-      <c r="AX4" s="62">
+      <c r="AR4" s="64"/>
+      <c r="AS4" s="64"/>
+      <c r="AT4" s="64"/>
+      <c r="AU4" s="64"/>
+      <c r="AV4" s="64"/>
+      <c r="AW4" s="65"/>
+      <c r="AX4" s="63">
         <f>AX5</f>
         <v>45803</v>
       </c>
-      <c r="AY4" s="63"/>
-      <c r="AZ4" s="63"/>
-      <c r="BA4" s="63"/>
-      <c r="BB4" s="63"/>
-      <c r="BC4" s="63"/>
-      <c r="BD4" s="64"/>
-      <c r="BE4" s="62">
+      <c r="AY4" s="64"/>
+      <c r="AZ4" s="64"/>
+      <c r="BA4" s="64"/>
+      <c r="BB4" s="64"/>
+      <c r="BC4" s="64"/>
+      <c r="BD4" s="65"/>
+      <c r="BE4" s="63">
         <f>BE5</f>
         <v>45810</v>
       </c>
-      <c r="BF4" s="63"/>
-      <c r="BG4" s="63"/>
-      <c r="BH4" s="63"/>
-      <c r="BI4" s="63"/>
-      <c r="BJ4" s="63"/>
-      <c r="BK4" s="64"/>
+      <c r="BF4" s="64"/>
+      <c r="BG4" s="64"/>
+      <c r="BH4" s="64"/>
+      <c r="BI4" s="64"/>
+      <c r="BJ4" s="64"/>
+      <c r="BK4" s="65"/>
     </row>
     <row r="5" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="31" t="s">
@@ -2549,7 +2552,7 @@
         <v>35</v>
       </c>
       <c r="C9" s="38" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="D9" s="51">
         <f>Début_Projet</f>
@@ -3385,12 +3388,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Image>
+    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
+    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </ImageTagsTaxHTField>
+    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3682,29 +3696,22 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Image>
-    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
-    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </ImageTagsTaxHTField>
-    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4A34E49-7289-4AEA-9593-4F55E04ADB10}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC3AD2E1-977A-4D4F-8EE8-D64B5FFADF75}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3731,13 +3738,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC3AD2E1-977A-4D4F-8EE8-D64B5FFADF75}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4A34E49-7289-4AEA-9593-4F55E04ADB10}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>